<commit_message>
cek log masing" file aja, agak lupa apa aja yang berubah, yang jelas nambah logo dinamik di unduhan lol
</commit_message>
<xml_diff>
--- a/docs/List Panitia/panitiafull[edit].xlsx
+++ b/docs/List Panitia/panitiafull[edit].xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DINAMIK\DINAMIK 12\PANITIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\DINAMIK12\docs\List Panitia\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9480" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9480" windowHeight="4635" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="283">
   <si>
     <t>Rijaalul Ummam Haryono</t>
   </si>
@@ -683,13 +683,205 @@
   </si>
   <si>
     <t>Sita Kartina</t>
+  </si>
+  <si>
+    <t>ketuplak</t>
+  </si>
+  <si>
+    <t>acara</t>
+  </si>
+  <si>
+    <t>bendahara</t>
+  </si>
+  <si>
+    <t>dokumentasi</t>
+  </si>
+  <si>
+    <t>humas</t>
+  </si>
+  <si>
+    <t>publikasi</t>
+  </si>
+  <si>
+    <t>sponsor</t>
+  </si>
+  <si>
+    <t>danusbazaar</t>
+  </si>
+  <si>
+    <t>rlf</t>
+  </si>
+  <si>
+    <t>cspc</t>
+  </si>
+  <si>
+    <t>lca</t>
+  </si>
+  <si>
+    <t>lcw</t>
+  </si>
+  <si>
+    <t>otik</t>
+  </si>
+  <si>
+    <t>ldg</t>
+  </si>
+  <si>
+    <t>pca</t>
+  </si>
+  <si>
+    <t>felose</t>
+  </si>
+  <si>
+    <t>semnas</t>
+  </si>
+  <si>
+    <t>talkshow</t>
+  </si>
+  <si>
+    <t>dstar</t>
+  </si>
+  <si>
+    <t>kj</t>
+  </si>
+  <si>
+    <t>!ketuplak!</t>
+  </si>
+  <si>
+    <t>!acara!</t>
+  </si>
+  <si>
+    <t>!bendahara!</t>
+  </si>
+  <si>
+    <t>!dokumentasi!</t>
+  </si>
+  <si>
+    <t>!humas!</t>
+  </si>
+  <si>
+    <t>!publikasi!</t>
+  </si>
+  <si>
+    <t>!sponsor!</t>
+  </si>
+  <si>
+    <t>!danusbazaar!</t>
+  </si>
+  <si>
+    <t>!rlf!</t>
+  </si>
+  <si>
+    <t>!cspc!</t>
+  </si>
+  <si>
+    <t>!lca!</t>
+  </si>
+  <si>
+    <t>!lcw!</t>
+  </si>
+  <si>
+    <t>!otik!</t>
+  </si>
+  <si>
+    <t>!ldg!</t>
+  </si>
+  <si>
+    <t>!pca!</t>
+  </si>
+  <si>
+    <t>!felose!</t>
+  </si>
+  <si>
+    <t>!semnas!</t>
+  </si>
+  <si>
+    <t>!talkshow!</t>
+  </si>
+  <si>
+    <t>!dstar!</t>
+  </si>
+  <si>
+    <t>!kj!</t>
+  </si>
+  <si>
+    <t>workshop</t>
+  </si>
+  <si>
+    <t>!workshop!</t>
+  </si>
+  <si>
+    <t>Divisi</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Workshop (?)</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>Tidak digunakan</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Verifikasi pembayaran peserta tim &amp; lomba</t>
+  </si>
+  <si>
+    <t>Sama dengan acara</t>
+  </si>
+  <si>
+    <t>Status Pengembangan</t>
+  </si>
+  <si>
+    <t>Manajemen berita &amp; galeri</t>
+  </si>
+  <si>
+    <t>Penyimpanan link berkas masih dalam pengembangan</t>
+  </si>
+  <si>
+    <t>Masih dalam pengembangan, galeri dalam bentuk IG API</t>
+  </si>
+  <si>
+    <t>Pesan masuk via web, membalas via web yang diteruskan ke email</t>
+  </si>
+  <si>
+    <t>Masih dalam pengembangan</t>
+  </si>
+  <si>
+    <t>Pendataan untuk bazaar</t>
+  </si>
+  <si>
+    <t>Pendataan sponsor, pemasangan sponsor di web akan menyesuaikan data disini</t>
+  </si>
+  <si>
+    <t>Mengubah deskripsi acara, buka/tutup pendaftaran, melihat semua daftar tim dan berkasnya (berupa link)</t>
+  </si>
+  <si>
+    <t>Selesai</t>
+  </si>
+  <si>
+    <t>Progress: Melihat anggota suatu tim</t>
+  </si>
+  <si>
+    <t>Progress: Berita di home, tombol share di detail berita, galeri (Instagram API)</t>
+  </si>
+  <si>
+    <t>Sama dengan acara, peserta bisa submit link berkas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -737,8 +929,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="29">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -907,8 +1112,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -989,11 +1206,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1536,11 +1774,140 @@
     <xf numFmtId="0" fontId="4" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="60% - Accent5" xfId="1" builtinId="48"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1551,6 +1918,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C2:G23" totalsRowShown="0" headerRowDxfId="6" dataDxfId="0" tableBorderDxfId="7" dataCellStyle="60% - Accent5">
+  <autoFilter ref="C2:G23"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Divisi" dataDxfId="5" dataCellStyle="60% - Accent5"/>
+    <tableColumn id="2" name="Username" dataDxfId="4" dataCellStyle="60% - Accent5"/>
+    <tableColumn id="3" name="Password" dataDxfId="3" dataCellStyle="60% - Accent5"/>
+    <tableColumn id="4" name="Keterangan" dataDxfId="2"/>
+    <tableColumn id="5" name="Status Pengembangan" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1816,10 +2197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E170"/>
+  <dimension ref="A1:J170"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="B1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1829,9 +2210,13 @@
     <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="172" t="s">
         <v>188</v>
       </c>
@@ -1846,7 +2231,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="169">
         <v>1</v>
       </c>
@@ -1859,8 +2244,26 @@
       <c r="D2" s="171" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="170" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="171">
+        <v>1405139</v>
+      </c>
+      <c r="H2" s="171" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="182" t="s">
+        <v>219</v>
+      </c>
+      <c r="J2" s="182" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <v>2</v>
       </c>
@@ -1873,8 +2276,26 @@
       <c r="D3" s="29" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="29">
+        <v>1404070</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="183" t="s">
+        <v>220</v>
+      </c>
+      <c r="J3" s="183" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <v>3</v>
       </c>
@@ -1887,8 +2308,26 @@
       <c r="D4" s="29" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>218</v>
+      </c>
+      <c r="G4" s="168">
+        <v>1406140</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>221</v>
+      </c>
+      <c r="J4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="33">
         <v>4</v>
       </c>
@@ -1901,8 +2340,26 @@
       <c r="D5" s="35" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="56">
+        <v>1505439</v>
+      </c>
+      <c r="H5" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>222</v>
+      </c>
+      <c r="J5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="33">
         <v>5</v>
       </c>
@@ -1915,8 +2372,26 @@
       <c r="D6" s="35" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="63">
+        <v>1401309</v>
+      </c>
+      <c r="H6" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>223</v>
+      </c>
+      <c r="J6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="40">
         <v>6</v>
       </c>
@@ -1929,8 +2404,26 @@
       <c r="D7" s="42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="20">
+        <v>1503677</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" t="s">
+        <v>224</v>
+      </c>
+      <c r="J7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="40">
         <v>7</v>
       </c>
@@ -1943,8 +2436,26 @@
       <c r="D8" s="42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8" s="94" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="95">
+        <v>1501393</v>
+      </c>
+      <c r="H8" s="96" t="s">
+        <v>179</v>
+      </c>
+      <c r="I8" t="s">
+        <v>225</v>
+      </c>
+      <c r="J8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="40">
         <v>8</v>
       </c>
@@ -1957,8 +2468,26 @@
       <c r="D9" s="42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="26">
+        <v>1400036</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="I9" t="s">
+        <v>226</v>
+      </c>
+      <c r="J9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="40">
         <v>9</v>
       </c>
@@ -1971,8 +2500,26 @@
       <c r="D10" s="42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10" s="136" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="137">
+        <v>1400793</v>
+      </c>
+      <c r="H10" s="137" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" t="s">
+        <v>227</v>
+      </c>
+      <c r="J10" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>10</v>
       </c>
@@ -1985,8 +2532,26 @@
       <c r="D11" s="42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11" s="107" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" s="108">
+        <v>1403356</v>
+      </c>
+      <c r="H11" s="108" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" t="s">
+        <v>228</v>
+      </c>
+      <c r="J11" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <v>11</v>
       </c>
@@ -1999,8 +2564,26 @@
       <c r="D12" s="42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12" s="176" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" s="177">
+        <v>1406424</v>
+      </c>
+      <c r="H12" s="177" t="s">
+        <v>92</v>
+      </c>
+      <c r="I12" t="s">
+        <v>229</v>
+      </c>
+      <c r="J12" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <v>12</v>
       </c>
@@ -2013,8 +2596,26 @@
       <c r="D13" s="42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="32">
+        <v>1401456</v>
+      </c>
+      <c r="H13" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" t="s">
+        <v>230</v>
+      </c>
+      <c r="J13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>13</v>
       </c>
@@ -2027,8 +2628,26 @@
       <c r="D14" s="42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="F14" s="102" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="103">
+        <v>1401788</v>
+      </c>
+      <c r="H14" s="103" t="s">
+        <v>211</v>
+      </c>
+      <c r="I14" t="s">
+        <v>231</v>
+      </c>
+      <c r="J14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <v>14</v>
       </c>
@@ -2041,8 +2660,26 @@
       <c r="D15" s="42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G15" s="17">
+        <v>1407273</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="I15" t="s">
+        <v>232</v>
+      </c>
+      <c r="J15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="40">
         <v>15</v>
       </c>
@@ -2055,8 +2692,26 @@
       <c r="D16" s="46" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16" s="120" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" s="121">
+        <v>1400707</v>
+      </c>
+      <c r="H16" s="121" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" t="s">
+        <v>233</v>
+      </c>
+      <c r="J16" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <v>16</v>
       </c>
@@ -2069,8 +2724,26 @@
       <c r="D17" s="23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17" s="115" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17" s="116">
+        <v>1404095</v>
+      </c>
+      <c r="H17" s="116" t="s">
+        <v>121</v>
+      </c>
+      <c r="I17" t="s">
+        <v>234</v>
+      </c>
+      <c r="J17" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
         <v>17</v>
       </c>
@@ -2083,8 +2756,26 @@
       <c r="D18" s="23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>17</v>
+      </c>
+      <c r="F18" s="110" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="111">
+        <v>1403294</v>
+      </c>
+      <c r="H18" s="111" t="s">
+        <v>132</v>
+      </c>
+      <c r="I18" t="s">
+        <v>235</v>
+      </c>
+      <c r="J18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="21">
         <v>18</v>
       </c>
@@ -2097,8 +2788,26 @@
       <c r="D19" s="23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>18</v>
+      </c>
+      <c r="F19" s="125" t="s">
+        <v>138</v>
+      </c>
+      <c r="G19" s="126">
+        <v>1405348</v>
+      </c>
+      <c r="H19" s="126" t="s">
+        <v>212</v>
+      </c>
+      <c r="I19" t="s">
+        <v>236</v>
+      </c>
+      <c r="J19" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
         <v>19</v>
       </c>
@@ -2111,8 +2820,26 @@
       <c r="D20" s="23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>19</v>
+      </c>
+      <c r="F20" s="87" t="s">
+        <v>143</v>
+      </c>
+      <c r="G20" s="88">
+        <v>1403441</v>
+      </c>
+      <c r="H20" s="88" t="s">
+        <v>144</v>
+      </c>
+      <c r="I20" t="s">
+        <v>237</v>
+      </c>
+      <c r="J20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="21">
         <v>20</v>
       </c>
@@ -2125,8 +2852,26 @@
       <c r="D21" s="23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21" s="165" t="s">
+        <v>217</v>
+      </c>
+      <c r="G21" s="166">
+        <v>1407206</v>
+      </c>
+      <c r="H21" s="167" t="s">
+        <v>213</v>
+      </c>
+      <c r="I21" t="s">
+        <v>238</v>
+      </c>
+      <c r="J21" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <v>21</v>
       </c>
@@ -2139,8 +2884,14 @@
       <c r="D22" s="50" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>259</v>
+      </c>
+      <c r="J22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <v>22</v>
       </c>
@@ -2154,7 +2905,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="54">
         <v>23</v>
       </c>
@@ -2168,7 +2919,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="54">
         <v>24</v>
       </c>
@@ -2182,7 +2933,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="54">
         <v>25</v>
       </c>
@@ -2196,7 +2947,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="54">
         <v>26</v>
       </c>
@@ -2210,7 +2961,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="54">
         <v>27</v>
       </c>
@@ -2224,7 +2975,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="54">
         <v>28</v>
       </c>
@@ -2238,7 +2989,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="54">
         <v>29</v>
       </c>
@@ -2252,7 +3003,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="61">
         <v>30</v>
       </c>
@@ -2266,7 +3017,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="61">
         <v>31</v>
       </c>
@@ -4579,14 +5330,440 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B43"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="81.7109375" customWidth="1"/>
+    <col min="7" max="7" width="44.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="184" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2" s="185" t="s">
+        <v>261</v>
+      </c>
+      <c r="D2" s="185" t="s">
+        <v>262</v>
+      </c>
+      <c r="E2" s="185" t="s">
+        <v>263</v>
+      </c>
+      <c r="F2" s="185" t="s">
+        <v>265</v>
+      </c>
+      <c r="G2" s="185" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="184">
+        <v>1</v>
+      </c>
+      <c r="C3" s="187" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="187" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3" s="187" t="s">
+        <v>239</v>
+      </c>
+      <c r="F3" s="188"/>
+      <c r="G3" s="189"/>
+    </row>
+    <row r="4" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="184">
+        <v>2</v>
+      </c>
+      <c r="C4" s="186" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="186" t="s">
+        <v>220</v>
+      </c>
+      <c r="E4" s="186" t="s">
+        <v>240</v>
+      </c>
+      <c r="F4" s="190" t="s">
+        <v>278</v>
+      </c>
+      <c r="G4" s="191" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="184">
+        <v>3</v>
+      </c>
+      <c r="C5" s="186" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="186" t="s">
+        <v>221</v>
+      </c>
+      <c r="E5" s="186" t="s">
+        <v>241</v>
+      </c>
+      <c r="F5" s="190" t="s">
+        <v>268</v>
+      </c>
+      <c r="G5" s="192"/>
+    </row>
+    <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="184">
+        <v>4</v>
+      </c>
+      <c r="C6" s="186" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="186" t="s">
+        <v>222</v>
+      </c>
+      <c r="E6" s="186" t="s">
+        <v>242</v>
+      </c>
+      <c r="F6" s="190" t="s">
+        <v>271</v>
+      </c>
+      <c r="G6" s="191" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="184">
+        <v>5</v>
+      </c>
+      <c r="C7" s="186" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="186" t="s">
+        <v>223</v>
+      </c>
+      <c r="E7" s="186" t="s">
+        <v>243</v>
+      </c>
+      <c r="F7" s="190" t="s">
+        <v>274</v>
+      </c>
+      <c r="G7" s="191" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="184">
+        <v>6</v>
+      </c>
+      <c r="C8" s="186" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="186" t="s">
+        <v>224</v>
+      </c>
+      <c r="E8" s="186" t="s">
+        <v>244</v>
+      </c>
+      <c r="F8" s="190" t="s">
+        <v>271</v>
+      </c>
+      <c r="G8" s="191" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="184">
+        <v>7</v>
+      </c>
+      <c r="C9" s="186" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" s="186" t="s">
+        <v>225</v>
+      </c>
+      <c r="E9" s="186" t="s">
+        <v>245</v>
+      </c>
+      <c r="F9" s="190" t="s">
+        <v>277</v>
+      </c>
+      <c r="G9" s="191" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="184">
+        <v>8</v>
+      </c>
+      <c r="C10" s="186" t="s">
+        <v>210</v>
+      </c>
+      <c r="D10" s="186" t="s">
+        <v>226</v>
+      </c>
+      <c r="E10" s="186" t="s">
+        <v>246</v>
+      </c>
+      <c r="F10" s="190" t="s">
+        <v>276</v>
+      </c>
+      <c r="G10" s="191" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="184">
+        <v>9</v>
+      </c>
+      <c r="C11" s="186" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="186" t="s">
+        <v>227</v>
+      </c>
+      <c r="E11" s="186" t="s">
+        <v>247</v>
+      </c>
+      <c r="F11" s="190" t="s">
+        <v>269</v>
+      </c>
+      <c r="G11" s="191"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="184">
+        <v>10</v>
+      </c>
+      <c r="C12" s="186" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="186" t="s">
+        <v>228</v>
+      </c>
+      <c r="E12" s="186" t="s">
+        <v>248</v>
+      </c>
+      <c r="F12" s="190" t="s">
+        <v>269</v>
+      </c>
+      <c r="G12" s="191"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="184">
+        <v>11</v>
+      </c>
+      <c r="C13" s="186" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="186" t="s">
+        <v>229</v>
+      </c>
+      <c r="E13" s="186" t="s">
+        <v>249</v>
+      </c>
+      <c r="F13" s="190" t="s">
+        <v>282</v>
+      </c>
+      <c r="G13" s="191"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="184">
+        <v>12</v>
+      </c>
+      <c r="C14" s="186" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="186" t="s">
+        <v>230</v>
+      </c>
+      <c r="E14" s="186" t="s">
+        <v>250</v>
+      </c>
+      <c r="F14" s="190" t="s">
+        <v>282</v>
+      </c>
+      <c r="G14" s="191"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="184">
+        <v>13</v>
+      </c>
+      <c r="C15" s="186" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" s="186" t="s">
+        <v>231</v>
+      </c>
+      <c r="E15" s="186" t="s">
+        <v>251</v>
+      </c>
+      <c r="F15" s="190" t="s">
+        <v>269</v>
+      </c>
+      <c r="G15" s="191"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="184">
+        <v>14</v>
+      </c>
+      <c r="C16" s="186" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="186" t="s">
+        <v>232</v>
+      </c>
+      <c r="E16" s="186" t="s">
+        <v>252</v>
+      </c>
+      <c r="F16" s="190" t="s">
+        <v>282</v>
+      </c>
+      <c r="G16" s="191"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="184">
+        <v>15</v>
+      </c>
+      <c r="C17" s="186" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="186" t="s">
+        <v>233</v>
+      </c>
+      <c r="E17" s="186" t="s">
+        <v>253</v>
+      </c>
+      <c r="F17" s="190" t="s">
+        <v>269</v>
+      </c>
+      <c r="G17" s="191"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="184">
+        <v>16</v>
+      </c>
+      <c r="C18" s="186" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="186" t="s">
+        <v>234</v>
+      </c>
+      <c r="E18" s="186" t="s">
+        <v>254</v>
+      </c>
+      <c r="F18" s="190" t="s">
+        <v>269</v>
+      </c>
+      <c r="G18" s="191"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="184">
+        <v>17</v>
+      </c>
+      <c r="C19" s="186" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="186" t="s">
+        <v>235</v>
+      </c>
+      <c r="E19" s="186" t="s">
+        <v>255</v>
+      </c>
+      <c r="F19" s="190" t="s">
+        <v>269</v>
+      </c>
+      <c r="G19" s="191"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="184">
+        <v>18</v>
+      </c>
+      <c r="C20" s="186" t="s">
+        <v>212</v>
+      </c>
+      <c r="D20" s="186" t="s">
+        <v>236</v>
+      </c>
+      <c r="E20" s="186" t="s">
+        <v>256</v>
+      </c>
+      <c r="F20" s="190" t="s">
+        <v>269</v>
+      </c>
+      <c r="G20" s="191"/>
+    </row>
+    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="184">
+        <v>19</v>
+      </c>
+      <c r="C21" s="186" t="s">
+        <v>144</v>
+      </c>
+      <c r="D21" s="186" t="s">
+        <v>237</v>
+      </c>
+      <c r="E21" s="186" t="s">
+        <v>257</v>
+      </c>
+      <c r="F21" s="190" t="s">
+        <v>269</v>
+      </c>
+      <c r="G21" s="191" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="184">
+        <v>20</v>
+      </c>
+      <c r="C22" s="186" t="s">
+        <v>213</v>
+      </c>
+      <c r="D22" s="186" t="s">
+        <v>238</v>
+      </c>
+      <c r="E22" s="186" t="s">
+        <v>258</v>
+      </c>
+      <c r="F22" s="190" t="s">
+        <v>269</v>
+      </c>
+      <c r="G22" s="191"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="184">
+        <v>21</v>
+      </c>
+      <c r="C23" s="186" t="s">
+        <v>264</v>
+      </c>
+      <c r="D23" s="186" t="s">
+        <v>259</v>
+      </c>
+      <c r="E23" s="186" t="s">
+        <v>260</v>
+      </c>
+      <c r="F23" s="190" t="s">
+        <v>266</v>
+      </c>
+      <c r="G23" s="191" t="s">
+        <v>279</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>